<commit_message>
Fix and added 2 parametric tests. Added rank and sign test
</commit_message>
<xml_diff>
--- a/tests/test_files/test_stocks_withevents.xlsx
+++ b/tests/test_files/test_stocks_withevents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="28455" windowHeight="11010"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="23280" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Precios" sheetId="1" r:id="rId1"/>
@@ -382,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A482" workbookViewId="0">
-      <selection activeCell="E511" sqref="E511"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="M510" sqref="M510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4660,7 +4660,7 @@
         <v>40877</v>
       </c>
       <c r="B252" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C252" s="2">
         <v>21.91</v>
@@ -4694,7 +4694,7 @@
         <v>40875</v>
       </c>
       <c r="B254" s="3">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="C254" s="2">
         <v>20.65</v>
@@ -4711,7 +4711,7 @@
         <v>40872</v>
       </c>
       <c r="B255" s="3">
-        <v>3.85</v>
+        <v>2.5</v>
       </c>
       <c r="C255" s="2">
         <v>19</v>
@@ -4728,7 +4728,7 @@
         <v>40870</v>
       </c>
       <c r="B256" s="3">
-        <v>3.95</v>
+        <v>2</v>
       </c>
       <c r="C256" s="2">
         <v>19.059999999999999</v>
@@ -4745,7 +4745,7 @@
         <v>40869</v>
       </c>
       <c r="B257" s="3">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="C257" s="2">
         <v>19.79</v>
@@ -4762,7 +4762,7 @@
         <v>40868</v>
       </c>
       <c r="B258" s="3">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="C258" s="2">
         <v>20.350000000000001</v>
@@ -4779,7 +4779,7 @@
         <v>40865</v>
       </c>
       <c r="B259" s="3">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="C259" s="2">
         <v>21.12</v>
@@ -4796,7 +4796,7 @@
         <v>40864</v>
       </c>
       <c r="B260" s="3">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="C260" s="2">
         <v>21.16</v>
@@ -4813,7 +4813,7 @@
         <v>40863</v>
       </c>
       <c r="B261" s="3">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="C261" s="2">
         <v>21.11</v>
@@ -8913,10 +8913,10 @@
         <v>1.94</v>
       </c>
       <c r="C502" s="3">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D502" s="3">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E502">
         <v>499</v>
@@ -8930,10 +8930,10 @@
         <v>1.97</v>
       </c>
       <c r="C503" s="3">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D503" s="3">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E503">
         <v>500</v>
@@ -8947,10 +8947,10 @@
         <v>1.93</v>
       </c>
       <c r="C504" s="3">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D504" s="3">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E504">
         <v>501</v>
@@ -8964,10 +8964,10 @@
         <v>1.9</v>
       </c>
       <c r="C505" s="3">
-        <v>46.5</v>
+        <v>27</v>
       </c>
       <c r="D505" s="3">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="E505">
         <v>502</v>
@@ -8981,10 +8981,10 @@
         <v>1.92</v>
       </c>
       <c r="C506" s="3">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D506" s="3">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E506">
         <v>503</v>
@@ -8998,10 +8998,10 @@
         <v>1.98</v>
       </c>
       <c r="C507" s="3">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D507" s="3">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="E507">
         <v>504</v>
@@ -9015,10 +9015,10 @@
         <v>1.92</v>
       </c>
       <c r="C508" s="3">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D508" s="3">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="E508">
         <v>505</v>
@@ -9032,10 +9032,10 @@
         <v>1.86</v>
       </c>
       <c r="C509" s="3">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D509" s="3">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E509">
         <v>506</v>
@@ -9049,10 +9049,10 @@
         <v>1.91</v>
       </c>
       <c r="C510" s="3">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D510" s="3">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E510">
         <v>507</v>
@@ -9066,10 +9066,10 @@
         <v>1.9</v>
       </c>
       <c r="C511" s="3">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D511" s="3">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E511">
         <v>508</v>

</xml_diff>